<commit_message>
add cancel button to interviews list and init db for applierRejectReason
</commit_message>
<xml_diff>
--- a/test/client/e2e test cases.xlsx
+++ b/test/client/e2e test cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14120" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20300" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="未登录" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3182" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3266" uniqueCount="759">
   <si>
     <t>步骤</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2462,441 +2462,509 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>interviews list 11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews list 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews offer 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews offer 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在interviews offer 2中点击搜索按钮后，点击清空按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews offer 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews offer 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在interviews offer 4中点击搜索按钮后，点击清空按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews offer 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboards 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboards 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboards 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在interviews onboards 2中点击搜索按钮后，点击清空按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboards 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboards 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboards 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboards 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboards 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboards 9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboards 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboards 11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在interviews onboards 10中点击搜索按钮后，点击清空按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在界面勾选记住我，输入正确用户名和密码登陆,登陆后退出浏览器，再次打开浏览器。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开网站，应可以直接进入主页/today</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应进入/login登陆界面，要求登陆后才能进入主页/today</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在界面取消勾选记住我，输入正确用户名和密码登陆。登陆后退出浏览器，再次打开浏览器，打开网站。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码不足六位不能点击按钮。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forgot3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码不足六位不能点击按钮。若重置链接无效，显示“重置链接无效”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forgot4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>若重置链接有效，显示“密码重置成功”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在forgot3中重置密码后，打开/login页面，用重置后的密码登陆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应能成功登陆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forgot5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>激活成功则显示“您的注册已激活，请使用邮箱和密码登陆”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在activate1中成功激活邮箱后，用注册的邮箱和密码登陆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应能成功登陆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>激活失败则显示“您的注册激活失败。可能因为该公司或邮箱已注册。”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activate3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activate2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activate4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在activate3中激活邮箱失败后，用注册的邮箱和密码登陆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应能不能成功登陆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>窗口应关闭，并跳转到/resumes/:id页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条应不显示。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>底部pagination条应显示总计数和分页数，分页数=总计数/50。总计数为0时pagination条应不显示。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/interviews/reviews</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条应不显示。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条显示“没有可以显示的项”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条显示“没有可以显示的项”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条显示“没有可以显示的项”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条显示“没有可以显示的项”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条显示“没有可以显示的项”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>底部pagination条应显示总计数和分页数，分页数=总计数/50。总计数为0时pagination条应不显示。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/applications/pursued/:index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications pursued 13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications pursued 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在applications pursued 12中单击“预约面试按钮”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应弹出创建面试预约的窗口</t>
+  </si>
+  <si>
+    <t>应弹出创建面试预约的窗口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在applications pursued 12中单击“归档”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications pursued 14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications pursued 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在applications pursued 12中单击“返回”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应显示通过的简历列表，表项中包含应聘职位，性别，生日，应聘时间，最高学历和最近工作等信息。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该应聘者被放入人才库中，页面载入下一个简历，并回到页面顶部。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面应有“预约面试”，“归档”和“返回三个按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/applications/pursued/:index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回通过的简历列表页面/applications/pursued，并滚动到返回前/applications/pursued/:index所对应的应聘者所在的位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面应有“通过”，“归档”和“返回三个按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications undetermined 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications undetermined 13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications undetermined 14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications undetermined 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/applications/undetermined/:index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/applications/undetermined/:index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回待定的简历列表页面/applications/undetermined/，并滚动到返回前/applications/undetermined/:index所对应的应聘者所在的位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在applications undetermined 12中单击“归档”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在applications undetermined 12中单击“通过”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，单击列表项中“详细”按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，单击列表项中“归档”按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，点击应聘职位过滤项中的某一项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，点击年龄过滤项中的25-29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，点击学历过滤项中的本科</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，在搜索栏中输入“理工大学”，点击搜索按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该应聘者被放入通过列表中，页面载入下一个简历，并回到页面顶部。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，单击列表项中“归档”按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，点击应聘职位过滤项中的某一项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，点击年龄过滤项中的25-29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，在搜索栏中输入“理工大学”，点击搜索按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，点击学历过滤项中的本科</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，单击列表项中“详细”按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面应有“通过”，“待定”，“归档”和“返回三个按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications new 14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/applications/new/:index</t>
+  </si>
+  <si>
+    <t>/applications/new/:index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新应聘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications new 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在applications new 14中单击“通过”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications new 16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在applications new 14中单击“归档”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在applications new 14中单击“返回”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在applications undetermined 12中单击“返回”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在applications new 14中单击“待定”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该应聘者被放入待定列表中，页面载入下一个简历，并回到页面顶部。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications new 17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applications new 18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回待定的简历列表页面/applications/new/，并滚动到返回前/applications/new/:index所对应的应聘者所在的位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>在interviews list 9中点击接受按钮</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>interviews list 11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews list 12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews offer 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews offer 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在interviews offer 2中点击搜索按钮后，点击清空按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews offer 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews offer 4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在interviews offer 4中点击搜索按钮后，点击清空按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews offer 5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews onboards 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews onboards 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews onboards 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在interviews onboards 2中点击搜索按钮后，点击清空按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews onboards 4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews onboards 5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews onboards 6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews onboards 7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews onboards 8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews onboards 9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews onboards 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interviews onboards 11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在interviews onboards 10中点击搜索按钮后，点击清空按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在界面勾选记住我，输入正确用户名和密码登陆,登陆后退出浏览器，再次打开浏览器。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>打开网站，应可以直接进入主页/today</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>应进入/login登陆界面，要求登陆后才能进入主页/today</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在界面取消勾选记住我，输入正确用户名和密码登陆。登陆后退出浏览器，再次打开浏览器，打开网站。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>密码不足六位不能点击按钮。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>forgot3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>密码不足六位不能点击按钮。若重置链接无效，显示“重置链接无效”。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>forgot4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>若重置链接有效，显示“密码重置成功”。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在forgot3中重置密码后，打开/login页面，用重置后的密码登陆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>应能成功登陆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>forgot5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>激活成功则显示“您的注册已激活，请使用邮箱和密码登陆”。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在activate1中成功激活邮箱后，用注册的邮箱和密码登陆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>应能成功登陆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>激活失败则显示“您的注册激活失败。可能因为该公司或邮箱已注册。”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activate3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activate2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activate4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在activate3中激活邮箱失败后，用注册的邮箱和密码登陆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>应能不能成功登陆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>窗口应关闭，并跳转到/resumes/:id页面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条应不显示。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>底部pagination条应显示总计数和分页数，分页数=总计数/50。总计数为0时pagination条应不显示。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/interviews/reviews</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条应不显示。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条显示“没有可以显示的项”。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条显示“没有可以显示的项”。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条显示“没有可以显示的项”。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条显示“没有可以显示的项”。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>底部pagination条应显示总计数和分页数。总计数为0时pagination条显示“没有可以显示的项”。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>底部pagination条应显示总计数和分页数，分页数=总计数/50。总计数为0时pagination条应不显示。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/applications/pursued/:index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications pursued 13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications pursued 12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在applications pursued 12中单击“预约面试按钮”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>应弹出创建面试预约的窗口</t>
-  </si>
-  <si>
-    <t>应弹出创建面试预约的窗口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在applications pursued 12中单击“归档”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications pursued 14</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications pursued 15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在applications pursued 12中单击“返回”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>应显示通过的简历列表，表项中包含应聘职位，性别，生日，应聘时间，最高学历和最近工作等信息。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>该应聘者被放入人才库中，页面载入下一个简历，并回到页面顶部。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>页面应有“预约面试”，“归档”和“返回三个按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/applications/pursued/:index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返回通过的简历列表页面/applications/pursued，并滚动到返回前/applications/pursued/:index所对应的应聘者所在的位置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>页面应有“通过”，“归档”和“返回三个按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications undetermined 12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications undetermined 13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications undetermined 14</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications undetermined 15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/applications/undetermined/:index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/applications/undetermined/:index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返回待定的简历列表页面/applications/undetermined/，并滚动到返回前/applications/undetermined/:index所对应的应聘者所在的位置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在applications undetermined 12中单击“归档”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在applications undetermined 12中单击“通过”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，单击列表项中“详细”按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，单击列表项中“归档”按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，点击应聘职位过滤项中的某一项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，点击年龄过滤项中的25-29</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，点击学历过滤项中的本科</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“待定”子菜单，在搜索栏中输入“理工大学”，点击搜索按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>该应聘者被放入通过列表中，页面载入下一个简历，并回到页面顶部。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，单击列表项中“归档”按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，点击应聘职位过滤项中的某一项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，点击年龄过滤项中的25-29</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，在搜索栏中输入“理工大学”，点击搜索按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，点击学历过滤项中的本科</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，单击列表项中“详细”按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>页面应有“通过”，“待定”，“归档”和“返回三个按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications new 14</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/applications/new/:index</t>
-  </si>
-  <si>
-    <t>/applications/new/:index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新应聘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications new 15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在applications new 14中单击“通过”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications new 16</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在applications new 14中单击“归档”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在applications new 14中单击“返回”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在applications undetermined 12中单击“返回”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在applications new 14中单击“待定”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>该应聘者被放入待定列表中，页面载入下一个简历，并回到页面顶部。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications new 17</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applications new 18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返回待定的简历列表页面/applications/new/，并滚动到返回前/applications/new/:index所对应的应聘者所在的位置</t>
+    <t>interviews offer 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者接受按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应出现入职日期选择器，以及保存和取消按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews offer 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者接受按钮，选择一个入职日期，然后点击保存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者拒绝按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应出现选择拒绝原因下拉菜单，以及保存和取消按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者拒绝按钮，选择一个拒绝原因，然后点击保存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存成功，应聘者进入人才库中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者接受按钮，然后点击取消按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回“应聘者接受”和“应聘者接受”按钮界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews offer 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存成功，应聘者进入待入职列表中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews offer 9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews offer 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews offer 11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者拒绝按钮，然后点击取消按钮</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3039,8 +3107,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="677">
+  <cellStyleXfs count="693">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3784,7 +3868,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="677">
+  <cellStyles count="693">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -4123,6 +4207,14 @@
     <cellStyle name="超链接" xfId="671" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="673" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="691" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -4461,6 +4553,14 @@
     <cellStyle name="访问过的超链接" xfId="672" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="674" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="692" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4935,7 +5035,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4943,7 +5043,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4983,7 +5083,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4991,7 +5091,7 @@
         <v>21</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -5087,7 +5187,7 @@
         <v>21</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -5099,7 +5199,7 @@
         <v>6</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -5139,7 +5239,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -5151,7 +5251,7 @@
         <v>6</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -5183,7 +5283,7 @@
         <v>19</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -5191,7 +5291,7 @@
         <v>1</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -5203,7 +5303,7 @@
         <v>6</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -5243,7 +5343,7 @@
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -5339,7 +5439,7 @@
         <v>21</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -5347,7 +5447,7 @@
         <v>6</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -5379,7 +5479,7 @@
         <v>19</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -5387,7 +5487,7 @@
         <v>1</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -5395,7 +5495,7 @@
         <v>6</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -5435,7 +5535,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -5443,7 +5543,7 @@
         <v>6</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -5475,7 +5575,7 @@
         <v>19</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -5483,7 +5583,7 @@
         <v>1</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
   </sheetData>
@@ -6152,7 +6252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="A140" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
@@ -6720,7 +6820,7 @@
         <v>70</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="30">
@@ -6776,7 +6876,7 @@
         <v>70</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -6832,7 +6932,7 @@
         <v>70</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -6888,7 +6988,7 @@
         <v>70</v>
       </c>
       <c r="B102" s="17" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -6944,7 +7044,7 @@
         <v>70</v>
       </c>
       <c r="B110" s="17" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -6964,7 +7064,7 @@
         <v>6</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -6980,7 +7080,7 @@
         <v>82</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -6988,7 +7088,7 @@
         <v>68</v>
       </c>
       <c r="B116" s="17" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -7004,7 +7104,7 @@
         <v>70</v>
       </c>
       <c r="B118" s="17" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -7012,7 +7112,7 @@
         <v>71</v>
       </c>
       <c r="B119" s="17" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -7020,7 +7120,7 @@
         <v>6</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -7036,7 +7136,7 @@
         <v>82</v>
       </c>
       <c r="B123" s="17" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -7044,7 +7144,7 @@
         <v>68</v>
       </c>
       <c r="B124" s="17" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -7060,7 +7160,7 @@
         <v>70</v>
       </c>
       <c r="B126" s="17" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="30">
@@ -7068,7 +7168,7 @@
         <v>71</v>
       </c>
       <c r="B127" s="17" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -7076,7 +7176,7 @@
         <v>6</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -7092,7 +7192,7 @@
         <v>82</v>
       </c>
       <c r="B131" s="17" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -7100,7 +7200,7 @@
         <v>68</v>
       </c>
       <c r="B132" s="17" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -7116,7 +7216,7 @@
         <v>70</v>
       </c>
       <c r="B134" s="17" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="30">
@@ -7124,7 +7224,7 @@
         <v>71</v>
       </c>
       <c r="B135" s="17" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -7132,7 +7232,7 @@
         <v>6</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -7148,7 +7248,7 @@
         <v>82</v>
       </c>
       <c r="B139" s="17" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -7156,7 +7256,7 @@
         <v>68</v>
       </c>
       <c r="B140" s="17" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -7172,7 +7272,7 @@
         <v>70</v>
       </c>
       <c r="B142" s="17" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -7180,7 +7280,7 @@
         <v>71</v>
       </c>
       <c r="B143" s="17" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -7188,7 +7288,7 @@
         <v>66</v>
       </c>
       <c r="B145" s="20" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -7212,7 +7312,7 @@
         <v>68</v>
       </c>
       <c r="B148" s="17" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -7228,7 +7328,7 @@
         <v>70</v>
       </c>
       <c r="B150" s="17" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="30">
@@ -7236,7 +7336,7 @@
         <v>71</v>
       </c>
       <c r="B151" s="17" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -7624,7 +7724,7 @@
         <v>70</v>
       </c>
       <c r="B207" s="17" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="30">
@@ -7680,7 +7780,7 @@
         <v>70</v>
       </c>
       <c r="B215" s="17" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -7736,7 +7836,7 @@
         <v>70</v>
       </c>
       <c r="B223" s="17" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -7792,7 +7892,7 @@
         <v>70</v>
       </c>
       <c r="B231" s="17" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -7848,7 +7948,7 @@
         <v>70</v>
       </c>
       <c r="B239" s="17" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -7868,7 +7968,7 @@
         <v>6</v>
       </c>
       <c r="B242" s="14" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -7892,7 +7992,7 @@
         <v>68</v>
       </c>
       <c r="B245" s="17" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -7908,7 +8008,7 @@
         <v>70</v>
       </c>
       <c r="B247" s="17" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -7916,7 +8016,7 @@
         <v>71</v>
       </c>
       <c r="B248" s="17" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -7924,7 +8024,7 @@
         <v>6</v>
       </c>
       <c r="B250" s="14" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -7948,7 +8048,7 @@
         <v>68</v>
       </c>
       <c r="B253" s="17" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -7964,7 +8064,7 @@
         <v>70</v>
       </c>
       <c r="B255" s="17" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="30">
@@ -7972,7 +8072,7 @@
         <v>71</v>
       </c>
       <c r="B256" s="17" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -7980,7 +8080,7 @@
         <v>6</v>
       </c>
       <c r="B258" s="14" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -8004,7 +8104,7 @@
         <v>68</v>
       </c>
       <c r="B261" s="17" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -8020,7 +8120,7 @@
         <v>70</v>
       </c>
       <c r="B263" s="17" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -8028,7 +8128,7 @@
         <v>71</v>
       </c>
       <c r="B264" s="17" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -8036,7 +8136,7 @@
         <v>6</v>
       </c>
       <c r="B266" s="14" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -8060,7 +8160,7 @@
         <v>68</v>
       </c>
       <c r="B269" s="17" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -8076,7 +8176,7 @@
         <v>70</v>
       </c>
       <c r="B271" s="17" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="45">
@@ -8084,7 +8184,7 @@
         <v>71</v>
       </c>
       <c r="B272" s="17" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -8140,7 +8240,7 @@
         <v>1</v>
       </c>
       <c r="B280" s="18" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -8712,7 +8812,7 @@
         <v>6</v>
       </c>
       <c r="B363" s="14" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -8736,7 +8836,7 @@
         <v>68</v>
       </c>
       <c r="B366" s="17" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -8760,7 +8860,7 @@
         <v>71</v>
       </c>
       <c r="B369" s="17" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -8768,7 +8868,7 @@
         <v>6</v>
       </c>
       <c r="B371" s="14" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="372" spans="1:2">
@@ -8792,7 +8892,7 @@
         <v>68</v>
       </c>
       <c r="B374" s="17" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="375" spans="1:2">
@@ -8808,7 +8908,7 @@
         <v>70</v>
       </c>
       <c r="B376" s="17" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="377" spans="1:2">
@@ -8816,7 +8916,7 @@
         <v>71</v>
       </c>
       <c r="B377" s="17" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="379" spans="1:2">
@@ -8824,7 +8924,7 @@
         <v>6</v>
       </c>
       <c r="B379" s="14" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="380" spans="1:2">
@@ -8848,7 +8948,7 @@
         <v>68</v>
       </c>
       <c r="B382" s="17" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="383" spans="1:2">
@@ -8864,7 +8964,7 @@
         <v>70</v>
       </c>
       <c r="B384" s="17" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="385" spans="1:2">
@@ -8872,7 +8972,7 @@
         <v>71</v>
       </c>
       <c r="B385" s="17" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="387" spans="1:2">
@@ -8880,7 +8980,7 @@
         <v>6</v>
       </c>
       <c r="B387" s="14" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="388" spans="1:2">
@@ -8904,7 +9004,7 @@
         <v>68</v>
       </c>
       <c r="B390" s="17" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="391" spans="1:2">
@@ -8920,7 +9020,7 @@
         <v>70</v>
       </c>
       <c r="B392" s="17" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="393" spans="1:2" ht="30">
@@ -8928,7 +9028,7 @@
         <v>71</v>
       </c>
       <c r="B393" s="17" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
   </sheetData>
@@ -9745,7 +9845,7 @@
         <v>71</v>
       </c>
       <c r="B112" s="17" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -11237,7 +11337,7 @@
         <v>434</v>
       </c>
       <c r="B320" s="17" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -14855,10 +14955,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B344"/>
+  <dimension ref="A1:B392"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B331" sqref="B331"/>
+    <sheetView tabSelected="1" topLeftCell="A280" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="B292" sqref="B292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16297,7 +16397,7 @@
         <v>335</v>
       </c>
       <c r="B202" s="20" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -16353,7 +16453,7 @@
         <v>66</v>
       </c>
       <c r="B210" s="20" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -16393,7 +16493,7 @@
         <v>70</v>
       </c>
       <c r="B215" s="17" t="s">
-        <v>632</v>
+        <v>741</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="45">
@@ -16409,7 +16509,7 @@
         <v>66</v>
       </c>
       <c r="B218" s="20" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -16465,7 +16565,7 @@
         <v>66</v>
       </c>
       <c r="B226" s="20" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -16521,7 +16621,7 @@
         <v>66</v>
       </c>
       <c r="B234" s="20" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -16561,7 +16661,7 @@
         <v>70</v>
       </c>
       <c r="B239" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -16577,7 +16677,7 @@
         <v>66</v>
       </c>
       <c r="B242" s="20" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -16633,7 +16733,7 @@
         <v>66</v>
       </c>
       <c r="B250" s="20" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -16673,7 +16773,7 @@
         <v>70</v>
       </c>
       <c r="B255" s="17" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -16689,7 +16789,7 @@
         <v>66</v>
       </c>
       <c r="B258" s="20" t="s">
-        <v>643</v>
+        <v>742</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -16705,7 +16805,7 @@
         <v>82</v>
       </c>
       <c r="B260" s="17" t="s">
-        <v>342</v>
+        <v>137</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -16713,7 +16813,7 @@
         <v>68</v>
       </c>
       <c r="B261" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -16729,15 +16829,15 @@
         <v>70</v>
       </c>
       <c r="B263" s="17" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" ht="45">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
       <c r="A264" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B264" s="17" t="s">
-        <v>350</v>
+        <v>744</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -16745,7 +16845,7 @@
         <v>66</v>
       </c>
       <c r="B266" s="20" t="s">
-        <v>642</v>
+        <v>745</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -16761,7 +16861,7 @@
         <v>82</v>
       </c>
       <c r="B268" s="17" t="s">
-        <v>342</v>
+        <v>137</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -16769,7 +16869,7 @@
         <v>68</v>
       </c>
       <c r="B269" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -16785,7 +16885,7 @@
         <v>70</v>
       </c>
       <c r="B271" s="17" t="s">
-        <v>351</v>
+        <v>746</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -16793,7 +16893,7 @@
         <v>71</v>
       </c>
       <c r="B272" s="17" t="s">
-        <v>305</v>
+        <v>754</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -16801,7 +16901,7 @@
         <v>66</v>
       </c>
       <c r="B274" s="20" t="s">
-        <v>644</v>
+        <v>753</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -16817,7 +16917,7 @@
         <v>82</v>
       </c>
       <c r="B276" s="17" t="s">
-        <v>342</v>
+        <v>137</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -16825,7 +16925,7 @@
         <v>68</v>
       </c>
       <c r="B277" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -16836,12 +16936,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" ht="30">
       <c r="A279" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B279" s="17" t="s">
-        <v>645</v>
+        <v>751</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -16849,19 +16949,15 @@
         <v>71</v>
       </c>
       <c r="B280" s="17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2">
-      <c r="A281" s="7"/>
-      <c r="B281" s="17"/>
+        <v>752</v>
+      </c>
     </row>
     <row r="282" spans="1:2">
       <c r="A282" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B282" s="20" t="s">
-        <v>646</v>
+        <v>755</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -16877,7 +16973,7 @@
         <v>82</v>
       </c>
       <c r="B284" s="17" t="s">
-        <v>342</v>
+        <v>137</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -16885,7 +16981,7 @@
         <v>68</v>
       </c>
       <c r="B285" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -16896,32 +16992,28 @@
         <v>83</v>
       </c>
     </row>
-    <row r="287" spans="1:2" ht="30">
+    <row r="287" spans="1:2">
       <c r="A287" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B287" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" ht="30">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
       <c r="A288" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B288" s="17" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2">
-      <c r="A289" s="7"/>
-      <c r="B289" s="17"/>
+        <v>748</v>
+      </c>
     </row>
     <row r="290" spans="1:2">
       <c r="A290" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B290" s="20" t="s">
-        <v>647</v>
+        <v>756</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -16937,7 +17029,7 @@
         <v>82</v>
       </c>
       <c r="B292" s="17" t="s">
-        <v>342</v>
+        <v>137</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -16945,7 +17037,7 @@
         <v>68</v>
       </c>
       <c r="B293" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -16961,27 +17053,23 @@
         <v>70</v>
       </c>
       <c r="B295" s="17" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" ht="30">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2">
       <c r="A296" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B296" s="17" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2">
-      <c r="A297" s="7"/>
-      <c r="B297" s="17"/>
+        <v>750</v>
+      </c>
     </row>
     <row r="298" spans="1:2">
       <c r="A298" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B298" s="20" t="s">
-        <v>648</v>
+        <v>757</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -16997,7 +17085,7 @@
         <v>82</v>
       </c>
       <c r="B300" s="17" t="s">
-        <v>342</v>
+        <v>137</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -17005,7 +17093,7 @@
         <v>68</v>
       </c>
       <c r="B301" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -17021,7 +17109,7 @@
         <v>70</v>
       </c>
       <c r="B303" s="17" t="s">
-        <v>358</v>
+        <v>758</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -17029,7 +17117,7 @@
         <v>71</v>
       </c>
       <c r="B304" s="17" t="s">
-        <v>359</v>
+        <v>752</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -17037,7 +17125,7 @@
         <v>66</v>
       </c>
       <c r="B306" s="20" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -17072,32 +17160,28 @@
         <v>83</v>
       </c>
     </row>
-    <row r="311" spans="1:2" ht="30">
+    <row r="311" spans="1:2">
       <c r="A311" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B311" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" ht="45">
       <c r="A312" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B312" s="17" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2">
-      <c r="A313" s="7"/>
-      <c r="B313" s="17"/>
+        <v>350</v>
+      </c>
     </row>
     <row r="314" spans="1:2">
       <c r="A314" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B314" s="20" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -17137,7 +17221,7 @@
         <v>70</v>
       </c>
       <c r="B319" s="17" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -17145,7 +17229,7 @@
         <v>71</v>
       </c>
       <c r="B320" s="17" t="s">
-        <v>363</v>
+        <v>305</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -17153,7 +17237,7 @@
         <v>66</v>
       </c>
       <c r="B322" s="20" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -17188,12 +17272,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="30">
+    <row r="327" spans="1:2">
       <c r="A327" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B327" s="17" t="s">
-        <v>364</v>
+        <v>644</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -17201,7 +17285,7 @@
         <v>71</v>
       </c>
       <c r="B328" s="17" t="s">
-        <v>365</v>
+        <v>308</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -17213,7 +17297,7 @@
         <v>66</v>
       </c>
       <c r="B330" s="20" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -17253,23 +17337,27 @@
         <v>70</v>
       </c>
       <c r="B335" s="17" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" ht="30">
       <c r="A336" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B336" s="17" t="s">
-        <v>353</v>
-      </c>
+        <v>355</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2">
+      <c r="A337" s="7"/>
+      <c r="B337" s="17"/>
     </row>
     <row r="338" spans="1:2">
       <c r="A338" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B338" s="20" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -17304,19 +17392,367 @@
         <v>83</v>
       </c>
     </row>
-    <row r="343" spans="1:2">
+    <row r="343" spans="1:2" ht="30">
       <c r="A343" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B343" s="17" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="344" spans="1:2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" ht="30">
       <c r="A344" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B344" s="17" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2">
+      <c r="A345" s="7"/>
+      <c r="B345" s="17"/>
+    </row>
+    <row r="346" spans="1:2">
+      <c r="A346" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B346" s="20" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2">
+      <c r="A347" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B347" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2">
+      <c r="A348" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B348" s="17" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2">
+      <c r="A349" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B349" s="17" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2">
+      <c r="A350" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B350" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" ht="30">
+      <c r="A351" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B351" s="17" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2">
+      <c r="A352" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B352" s="17" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2">
+      <c r="A354" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B354" s="20" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2">
+      <c r="A355" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B355" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2">
+      <c r="A356" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B356" s="17" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2">
+      <c r="A357" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B357" s="17" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2">
+      <c r="A358" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B358" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" ht="30">
+      <c r="A359" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B359" s="17" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2">
+      <c r="A360" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B360" s="17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2">
+      <c r="A361" s="7"/>
+      <c r="B361" s="17"/>
+    </row>
+    <row r="362" spans="1:2">
+      <c r="A362" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B362" s="20" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2">
+      <c r="A363" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B363" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2">
+      <c r="A364" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B364" s="17" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2">
+      <c r="A365" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B365" s="17" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2">
+      <c r="A366" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B366" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" ht="30">
+      <c r="A367" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B367" s="17" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2">
+      <c r="A368" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B368" s="17" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2">
+      <c r="A370" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B370" s="20" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2">
+      <c r="A371" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B371" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2">
+      <c r="A372" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B372" s="17" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2">
+      <c r="A373" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B373" s="17" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2">
+      <c r="A374" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B374" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" ht="30">
+      <c r="A375" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B375" s="17" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2">
+      <c r="A376" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B376" s="17" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2">
+      <c r="A377" s="7"/>
+      <c r="B377" s="17"/>
+    </row>
+    <row r="378" spans="1:2">
+      <c r="A378" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B378" s="20" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2">
+      <c r="A379" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B379" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2">
+      <c r="A380" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B380" s="17" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2">
+      <c r="A381" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B381" s="17" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2">
+      <c r="A382" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B382" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" ht="30">
+      <c r="A383" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B383" s="17" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2">
+      <c r="A384" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B384" s="17" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2">
+      <c r="A386" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B386" s="20" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2">
+      <c r="A387" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B387" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2">
+      <c r="A388" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B388" s="17" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2">
+      <c r="A389" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B389" s="17" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2">
+      <c r="A390" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B390" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2">
+      <c r="A391" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B391" s="17" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2">
+      <c r="A392" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B392" s="17" t="s">
         <v>308</v>
       </c>
     </row>
@@ -17398,7 +17834,7 @@
         <v>71</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -17454,7 +17890,7 @@
         <v>71</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -17510,7 +17946,7 @@
         <v>71</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -17542,7 +17978,7 @@
         <v>68</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -17566,7 +18002,7 @@
         <v>71</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -17622,7 +18058,7 @@
         <v>71</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -17678,7 +18114,7 @@
         <v>71</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -17734,7 +18170,7 @@
         <v>71</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -17790,7 +18226,7 @@
         <v>71</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -17846,7 +18282,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -17902,7 +18338,7 @@
         <v>71</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -17926,7 +18362,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -17958,7 +18394,7 @@
         <v>71</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add validation for offer and onboards save button
</commit_message>
<xml_diff>
--- a/test/client/e2e test cases.xlsx
+++ b/test/client/e2e test cases.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3266" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3406" uniqueCount="781">
   <si>
     <t>步骤</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2912,46 +2912,54 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者接受按钮，选择一个入职日期，然后点击保存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者拒绝按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应出现选择拒绝原因下拉菜单，以及保存和取消按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者拒绝按钮，选择一个拒绝原因，然后点击保存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存成功，应聘者进入人才库中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者接受按钮，然后点击取消按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回“应聘者接受”和“应聘者接受”按钮界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存成功，应聘者进入待入职列表中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者拒绝按钮，然后点击取消按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未选择日期时，保存按钮应为disabled状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>interviews offer 7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者接受按钮，选择一个入职日期，然后点击保存</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者拒绝按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>应出现选择拒绝原因下拉菜单，以及保存和取消按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者拒绝按钮，选择一个拒绝原因，然后点击保存</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>保存成功，应聘者进入人才库中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者接受按钮，然后点击取消按钮</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返回“应聘者接受”和“应聘者接受”按钮界面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>interviews offer 8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>保存成功，应聘者进入待入职列表中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>interviews offer 9</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2964,7 +2972,75 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>在导航栏中点击面试菜单，点击通过子菜单,点击应聘者拒绝按钮，然后点击取消按钮</t>
+    <t>interviews offer 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews offer 13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/interviews/onboards</t>
+  </si>
+  <si>
+    <t>interviews onboard 10</t>
+  </si>
+  <si>
+    <t>interviews onboard 11</t>
+  </si>
+  <si>
+    <t>interviews onboard 12</t>
+  </si>
+  <si>
+    <t>interviews onboard 13</t>
+  </si>
+  <si>
+    <t>入职</t>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击入职子菜单,点击应聘者接受按钮</t>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击入职子菜单,点击应聘者接受按钮，选择一个入职日期，然后点击保存</t>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击入职子菜单,点击应聘者接受按钮，然后点击取消按钮</t>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击入职子菜单,点击应聘者拒绝按钮</t>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击入职子菜单,点击应聘者拒绝按钮，选择一个拒绝原因，然后点击保存</t>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击入职子菜单,点击应聘者拒绝按钮，然后点击取消按钮</t>
+  </si>
+  <si>
+    <t>interviews onboard 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboard 13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboard 14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interviews onboard 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存成功，应聘者状态变为已入职，并从入职列表中消失</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未选择拒绝原因时，保存按钮应为disabled状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击面试菜单，点击入职子菜单,点击应聘者拒绝按钮</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3107,8 +3183,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="693">
+  <cellStyleXfs count="701">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3868,7 +3952,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="693">
+  <cellStyles count="701">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -4215,6 +4299,10 @@
     <cellStyle name="超链接" xfId="687" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="689" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="699" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -4561,6 +4649,10 @@
     <cellStyle name="访问过的超链接" xfId="688" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="690" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="700" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -12091,7 +12183,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14955,10 +15047,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B392"/>
+  <dimension ref="A1:B473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B292" sqref="B292"/>
+    <sheetView tabSelected="1" topLeftCell="A444" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="C453" sqref="C453"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16840,12 +16932,16 @@
         <v>744</v>
       </c>
     </row>
+    <row r="265" spans="1:2">
+      <c r="A265" s="7"/>
+      <c r="B265" s="17"/>
+    </row>
     <row r="266" spans="1:2">
       <c r="A266" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B266" s="20" t="s">
-        <v>745</v>
+        <v>755</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -16880,12 +16976,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="271" spans="1:2" ht="30">
+    <row r="271" spans="1:2">
       <c r="A271" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B271" s="17" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -16901,7 +16997,7 @@
         <v>66</v>
       </c>
       <c r="B274" s="20" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -16941,7 +17037,7 @@
         <v>70</v>
       </c>
       <c r="B279" s="17" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -16957,7 +17053,7 @@
         <v>66</v>
       </c>
       <c r="B282" s="20" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -16992,12 +17088,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" ht="30">
       <c r="A287" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B287" s="17" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -17005,7 +17101,7 @@
         <v>71</v>
       </c>
       <c r="B288" s="17" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -17013,7 +17109,7 @@
         <v>66</v>
       </c>
       <c r="B290" s="20" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -17048,12 +17144,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="295" spans="1:2" ht="30">
+    <row r="295" spans="1:2">
       <c r="A295" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B295" s="17" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -17061,15 +17157,19 @@
         <v>71</v>
       </c>
       <c r="B296" s="17" t="s">
-        <v>750</v>
-      </c>
+        <v>747</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
+      <c r="A297" s="7"/>
+      <c r="B297" s="17"/>
     </row>
     <row r="298" spans="1:2">
       <c r="A298" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B298" s="20" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -17104,12 +17204,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="30">
+    <row r="303" spans="1:2">
       <c r="A303" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B303" s="17" t="s">
-        <v>758</v>
+        <v>746</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -17117,7 +17217,7 @@
         <v>71</v>
       </c>
       <c r="B304" s="17" t="s">
-        <v>752</v>
+        <v>779</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -17125,7 +17225,7 @@
         <v>66</v>
       </c>
       <c r="B306" s="20" t="s">
-        <v>642</v>
+        <v>760</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -17141,7 +17241,7 @@
         <v>82</v>
       </c>
       <c r="B308" s="17" t="s">
-        <v>342</v>
+        <v>137</v>
       </c>
     </row>
     <row r="309" spans="1:2">
@@ -17149,7 +17249,7 @@
         <v>68</v>
       </c>
       <c r="B309" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="310" spans="1:2">
@@ -17160,20 +17260,20 @@
         <v>83</v>
       </c>
     </row>
-    <row r="311" spans="1:2">
+    <row r="311" spans="1:2" ht="30">
       <c r="A311" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B311" s="17" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" ht="45">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2">
       <c r="A312" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B312" s="17" t="s">
-        <v>350</v>
+        <v>749</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -17181,7 +17281,7 @@
         <v>66</v>
       </c>
       <c r="B314" s="20" t="s">
-        <v>641</v>
+        <v>761</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -17197,7 +17297,7 @@
         <v>82</v>
       </c>
       <c r="B316" s="17" t="s">
-        <v>342</v>
+        <v>137</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -17205,7 +17305,7 @@
         <v>68</v>
       </c>
       <c r="B317" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -17221,7 +17321,7 @@
         <v>70</v>
       </c>
       <c r="B319" s="17" t="s">
-        <v>351</v>
+        <v>753</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -17229,7 +17329,7 @@
         <v>71</v>
       </c>
       <c r="B320" s="17" t="s">
-        <v>305</v>
+        <v>751</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -17237,7 +17337,7 @@
         <v>66</v>
       </c>
       <c r="B322" s="20" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -17277,27 +17377,23 @@
         <v>70</v>
       </c>
       <c r="B327" s="17" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" ht="45">
       <c r="A328" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B328" s="17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2">
-      <c r="A329" s="7"/>
-      <c r="B329" s="17"/>
+        <v>350</v>
+      </c>
     </row>
     <row r="330" spans="1:2">
       <c r="A330" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B330" s="20" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -17337,27 +17433,23 @@
         <v>70</v>
       </c>
       <c r="B335" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" ht="30">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
       <c r="A336" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B336" s="17" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="337" spans="1:2">
-      <c r="A337" s="7"/>
-      <c r="B337" s="17"/>
+        <v>305</v>
+      </c>
     </row>
     <row r="338" spans="1:2">
       <c r="A338" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B338" s="20" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -17392,20 +17484,20 @@
         <v>83</v>
       </c>
     </row>
-    <row r="343" spans="1:2" ht="30">
+    <row r="343" spans="1:2">
       <c r="A343" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B343" s="17" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="344" spans="1:2" ht="30">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2">
       <c r="A344" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B344" s="17" t="s">
-        <v>357</v>
+        <v>308</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -17417,7 +17509,7 @@
         <v>66</v>
       </c>
       <c r="B346" s="20" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -17457,23 +17549,27 @@
         <v>70</v>
       </c>
       <c r="B351" s="17" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="352" spans="1:2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" ht="30">
       <c r="A352" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B352" s="17" t="s">
-        <v>359</v>
-      </c>
+        <v>355</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2">
+      <c r="A353" s="7"/>
+      <c r="B353" s="17"/>
     </row>
     <row r="354" spans="1:2">
       <c r="A354" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B354" s="20" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -17513,15 +17609,15 @@
         <v>70</v>
       </c>
       <c r="B359" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="360" spans="1:2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" ht="30">
       <c r="A360" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B360" s="17" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -17533,7 +17629,7 @@
         <v>66</v>
       </c>
       <c r="B362" s="20" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -17573,7 +17669,7 @@
         <v>70</v>
       </c>
       <c r="B367" s="17" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="368" spans="1:2">
@@ -17581,7 +17677,7 @@
         <v>71</v>
       </c>
       <c r="B368" s="17" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="370" spans="1:2">
@@ -17589,7 +17685,7 @@
         <v>66</v>
       </c>
       <c r="B370" s="20" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -17629,7 +17725,7 @@
         <v>70</v>
       </c>
       <c r="B375" s="17" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="376" spans="1:2">
@@ -17637,7 +17733,7 @@
         <v>71</v>
       </c>
       <c r="B376" s="17" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="377" spans="1:2">
@@ -17649,7 +17745,7 @@
         <v>66</v>
       </c>
       <c r="B378" s="20" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="379" spans="1:2">
@@ -17689,7 +17785,7 @@
         <v>70</v>
       </c>
       <c r="B383" s="17" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
     </row>
     <row r="384" spans="1:2">
@@ -17697,7 +17793,7 @@
         <v>71</v>
       </c>
       <c r="B384" s="17" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
     </row>
     <row r="386" spans="1:2">
@@ -17705,7 +17801,7 @@
         <v>66</v>
       </c>
       <c r="B386" s="20" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="387" spans="1:2">
@@ -17740,12 +17836,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="391" spans="1:2">
+    <row r="391" spans="1:2" ht="30">
       <c r="A391" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B391" s="17" t="s">
-        <v>653</v>
+        <v>364</v>
       </c>
     </row>
     <row r="392" spans="1:2">
@@ -17753,7 +17849,579 @@
         <v>71</v>
       </c>
       <c r="B392" s="17" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2">
+      <c r="A393" s="7"/>
+      <c r="B393" s="17"/>
+    </row>
+    <row r="394" spans="1:2">
+      <c r="A394" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B394" s="20" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2">
+      <c r="A395" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B395" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2">
+      <c r="A396" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B396" s="17" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2">
+      <c r="A397" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B397" s="17" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2">
+      <c r="A398" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B398" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" ht="30">
+      <c r="A399" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B399" s="17" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2">
+      <c r="A400" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B400" s="17" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2">
+      <c r="A402" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B402" s="20" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2">
+      <c r="A403" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B403" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2">
+      <c r="A404" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B404" s="17" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2">
+      <c r="A405" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B405" s="17" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2">
+      <c r="A406" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B406" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2">
+      <c r="A407" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B407" s="17" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2">
+      <c r="A408" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B408" s="17" t="s">
         <v>308</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2">
+      <c r="A411" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B411" s="20" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2">
+      <c r="A412" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B412" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2">
+      <c r="A413" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B413" s="17" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2">
+      <c r="A414" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B414" s="17" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2">
+      <c r="A415" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B415" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2">
+      <c r="A416" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B416" s="17" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2">
+      <c r="A417" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B417" s="17" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2">
+      <c r="A418" s="7"/>
+      <c r="B418" s="17"/>
+    </row>
+    <row r="419" spans="1:2">
+      <c r="A419" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B419" s="20" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2">
+      <c r="A420" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B420" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2">
+      <c r="A421" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B421" s="17" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2">
+      <c r="A422" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B422" s="17" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2">
+      <c r="A423" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B423" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2">
+      <c r="A424" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B424" s="17" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2">
+      <c r="A425" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B425" s="17" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2">
+      <c r="A427" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B427" s="20" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2">
+      <c r="A428" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B428" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2">
+      <c r="A429" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B429" s="17" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2">
+      <c r="A430" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B430" s="17" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2">
+      <c r="A431" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B431" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" ht="30">
+      <c r="A432" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B432" s="17" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2">
+      <c r="A433" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B433" s="17" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2">
+      <c r="A435" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B435" s="20" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2">
+      <c r="A436" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B436" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2">
+      <c r="A437" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B437" s="17" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2">
+      <c r="A438" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B438" s="17" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2">
+      <c r="A439" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B439" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" ht="30">
+      <c r="A440" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B440" s="17" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2">
+      <c r="A441" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B441" s="17" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2">
+      <c r="A443" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B443" s="20" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2">
+      <c r="A444" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B444" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2">
+      <c r="A445" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B445" s="17" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2">
+      <c r="A446" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B446" s="17" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2">
+      <c r="A447" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B447" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2">
+      <c r="A448" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B448" s="17" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2">
+      <c r="A449" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B449" s="17" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2">
+      <c r="A450" s="7"/>
+      <c r="B450" s="17"/>
+    </row>
+    <row r="451" spans="1:2">
+      <c r="A451" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B451" s="20" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2">
+      <c r="A452" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B452" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2">
+      <c r="A453" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B453" s="17" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2">
+      <c r="A454" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B454" s="17" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2">
+      <c r="A455" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B455" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2">
+      <c r="A456" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B456" s="17" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2">
+      <c r="A457" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B457" s="17" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2">
+      <c r="A459" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B459" s="20" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2">
+      <c r="A460" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B460" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2">
+      <c r="A461" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B461" s="17" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2">
+      <c r="A462" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B462" s="17" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2">
+      <c r="A463" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B463" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" ht="30">
+      <c r="A464" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B464" s="17" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2">
+      <c r="A465" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B465" s="17" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2">
+      <c r="A467" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B467" s="20" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2">
+      <c r="A468" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B468" s="17" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2">
+      <c r="A469" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B469" s="17" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2">
+      <c r="A470" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B470" s="17" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2">
+      <c r="A471" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B471" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" ht="30">
+      <c r="A472" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B472" s="17" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2">
+      <c r="A473" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B473" s="17" t="s">
+        <v>751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix nav bar counts bug for application detail view button click
</commit_message>
<xml_diff>
--- a/test/client/e2e test cases.xlsx
+++ b/test/client/e2e test cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20300" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20300" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="未登录" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3406" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3406" uniqueCount="784">
   <si>
     <t>步骤</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2725,10 +2725,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>该应聘者被放入人才库中，页面载入下一个简历，并回到页面顶部。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>页面应有“预约面试”，“归档”和“返回三个按钮</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2805,10 +2801,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>该应聘者被放入通过列表中，页面载入下一个简历，并回到页面顶部。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>点击导航栏中的“应聘”菜单,然后点击“新应聘”子菜单，单击列表项中“归档”按钮</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2880,10 +2872,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>该应聘者被放入待定列表中，页面载入下一个简历，并回到页面顶部。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>applications new 17</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3041,6 +3029,30 @@
   </si>
   <si>
     <t>在导航栏中点击面试菜单，点击入职子菜单,点击应聘者拒绝按钮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该应聘者被放入通过列表中，页面载入下一个简历，并回到页面顶部。导航栏中“新应聘”子菜单计数值减一，“通过”子菜单计数值加一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该应聘者被放入待定列表中，页面载入下一个简历，并回到页面顶部。导航栏中“新应聘”子菜单计数值减一，“待定”子菜单计数值加一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该应聘者被放入人才库中，页面载入下一个简历，并回到页面顶部。导航栏中“新应聘”子菜单计数值减一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该应聘者被放入人才库中，页面载入下一个简历，并回到页面顶部。导航栏中“待定”子菜单计数值减一。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该应聘者被放入通过列表中，页面载入下一个简历，并回到页面顶部。导航栏中“待定”子菜单计数值减一，“通过”子菜单计数值加一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>该应聘者被放入人才库中，页面载入下一个简历，并回到页面顶部。导航栏中“通过”子菜单计数值减一。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3183,8 +3195,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="701">
+  <cellStyleXfs count="703">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3952,7 +3966,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="701">
+  <cellStyles count="703">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -4303,6 +4317,7 @@
     <cellStyle name="超链接" xfId="695" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="697" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="701" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -4653,6 +4668,7 @@
     <cellStyle name="访问过的超链接" xfId="696" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="698" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="702" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6344,8 +6360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E393"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F144" sqref="F144"/>
+    <sheetView tabSelected="1" topLeftCell="A362" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F376" sqref="F376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6912,7 +6928,7 @@
         <v>70</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="30">
@@ -6968,7 +6984,7 @@
         <v>70</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -7024,7 +7040,7 @@
         <v>70</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -7080,7 +7096,7 @@
         <v>70</v>
       </c>
       <c r="B102" s="17" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -7136,7 +7152,7 @@
         <v>70</v>
       </c>
       <c r="B110" s="17" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -7156,7 +7172,7 @@
         <v>6</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -7172,7 +7188,7 @@
         <v>82</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -7180,7 +7196,7 @@
         <v>68</v>
       </c>
       <c r="B116" s="17" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -7196,7 +7212,7 @@
         <v>70</v>
       </c>
       <c r="B118" s="17" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -7204,7 +7220,7 @@
         <v>71</v>
       </c>
       <c r="B119" s="17" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -7212,7 +7228,7 @@
         <v>6</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -7228,7 +7244,7 @@
         <v>82</v>
       </c>
       <c r="B123" s="17" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -7236,7 +7252,7 @@
         <v>68</v>
       </c>
       <c r="B124" s="17" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -7252,15 +7268,15 @@
         <v>70</v>
       </c>
       <c r="B126" s="17" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="30">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="45">
       <c r="A127" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B127" s="17" t="s">
-        <v>718</v>
+        <v>778</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -7268,7 +7284,7 @@
         <v>6</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -7284,7 +7300,7 @@
         <v>82</v>
       </c>
       <c r="B131" s="17" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -7292,7 +7308,7 @@
         <v>68</v>
       </c>
       <c r="B132" s="17" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -7308,15 +7324,15 @@
         <v>70</v>
       </c>
       <c r="B134" s="17" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="30">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="45">
       <c r="A135" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B135" s="17" t="s">
-        <v>737</v>
+        <v>779</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -7324,7 +7340,7 @@
         <v>6</v>
       </c>
       <c r="B137" s="14" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -7340,7 +7356,7 @@
         <v>82</v>
       </c>
       <c r="B139" s="17" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -7348,7 +7364,7 @@
         <v>68</v>
       </c>
       <c r="B140" s="17" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -7364,15 +7380,15 @@
         <v>70</v>
       </c>
       <c r="B142" s="17" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="30">
       <c r="A143" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B143" s="17" t="s">
-        <v>698</v>
+        <v>780</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -7380,7 +7396,7 @@
         <v>66</v>
       </c>
       <c r="B145" s="20" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -7404,7 +7420,7 @@
         <v>68</v>
       </c>
       <c r="B148" s="17" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -7420,7 +7436,7 @@
         <v>70</v>
       </c>
       <c r="B150" s="17" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="30">
@@ -7428,7 +7444,7 @@
         <v>71</v>
       </c>
       <c r="B151" s="17" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -7816,7 +7832,7 @@
         <v>70</v>
       </c>
       <c r="B207" s="17" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="30">
@@ -7872,7 +7888,7 @@
         <v>70</v>
       </c>
       <c r="B215" s="17" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -7928,7 +7944,7 @@
         <v>70</v>
       </c>
       <c r="B223" s="17" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -7984,7 +8000,7 @@
         <v>70</v>
       </c>
       <c r="B231" s="17" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -8040,7 +8056,7 @@
         <v>70</v>
       </c>
       <c r="B239" s="17" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -8060,7 +8076,7 @@
         <v>6</v>
       </c>
       <c r="B242" s="14" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -8084,7 +8100,7 @@
         <v>68</v>
       </c>
       <c r="B245" s="17" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -8100,7 +8116,7 @@
         <v>70</v>
       </c>
       <c r="B247" s="17" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -8108,7 +8124,7 @@
         <v>71</v>
       </c>
       <c r="B248" s="17" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -8116,7 +8132,7 @@
         <v>6</v>
       </c>
       <c r="B250" s="14" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -8140,7 +8156,7 @@
         <v>68</v>
       </c>
       <c r="B253" s="17" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -8156,15 +8172,15 @@
         <v>70</v>
       </c>
       <c r="B255" s="17" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" ht="30">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" ht="45">
       <c r="A256" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B256" s="17" t="s">
-        <v>718</v>
+        <v>782</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -8172,7 +8188,7 @@
         <v>6</v>
       </c>
       <c r="B258" s="14" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -8196,7 +8212,7 @@
         <v>68</v>
       </c>
       <c r="B261" s="17" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -8212,15 +8228,15 @@
         <v>70</v>
       </c>
       <c r="B263" s="17" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" ht="30">
       <c r="A264" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B264" s="17" t="s">
-        <v>698</v>
+        <v>781</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -8228,7 +8244,7 @@
         <v>6</v>
       </c>
       <c r="B266" s="14" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -8252,7 +8268,7 @@
         <v>68</v>
       </c>
       <c r="B269" s="17" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -8268,7 +8284,7 @@
         <v>70</v>
       </c>
       <c r="B271" s="17" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="45">
@@ -8276,7 +8292,7 @@
         <v>71</v>
       </c>
       <c r="B272" s="17" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -8952,7 +8968,7 @@
         <v>71</v>
       </c>
       <c r="B369" s="17" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -9059,12 +9075,12 @@
         <v>693</v>
       </c>
     </row>
-    <row r="385" spans="1:2">
+    <row r="385" spans="1:2" ht="30">
       <c r="A385" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B385" s="17" t="s">
-        <v>698</v>
+        <v>783</v>
       </c>
     </row>
     <row r="387" spans="1:2">
@@ -9096,7 +9112,7 @@
         <v>68</v>
       </c>
       <c r="B390" s="17" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="391" spans="1:2">
@@ -9120,7 +9136,7 @@
         <v>71</v>
       </c>
       <c r="B393" s="17" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>
@@ -15049,7 +15065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A444" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView topLeftCell="A444" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
       <selection activeCell="C453" sqref="C453"/>
     </sheetView>
   </sheetViews>
@@ -16585,7 +16601,7 @@
         <v>70</v>
       </c>
       <c r="B215" s="17" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="45">
@@ -16881,7 +16897,7 @@
         <v>66</v>
       </c>
       <c r="B258" s="20" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -16921,7 +16937,7 @@
         <v>70</v>
       </c>
       <c r="B263" s="17" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -16929,7 +16945,7 @@
         <v>71</v>
       </c>
       <c r="B264" s="17" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -16941,7 +16957,7 @@
         <v>66</v>
       </c>
       <c r="B266" s="20" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -16981,7 +16997,7 @@
         <v>70</v>
       </c>
       <c r="B271" s="17" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -16989,7 +17005,7 @@
         <v>71</v>
       </c>
       <c r="B272" s="17" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -16997,7 +17013,7 @@
         <v>66</v>
       </c>
       <c r="B274" s="20" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -17037,7 +17053,7 @@
         <v>70</v>
       </c>
       <c r="B279" s="17" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -17045,7 +17061,7 @@
         <v>71</v>
       </c>
       <c r="B280" s="17" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -17053,7 +17069,7 @@
         <v>66</v>
       </c>
       <c r="B282" s="20" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -17093,7 +17109,7 @@
         <v>70</v>
       </c>
       <c r="B287" s="17" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -17101,7 +17117,7 @@
         <v>71</v>
       </c>
       <c r="B288" s="17" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -17109,7 +17125,7 @@
         <v>66</v>
       </c>
       <c r="B290" s="20" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -17149,7 +17165,7 @@
         <v>70</v>
       </c>
       <c r="B295" s="17" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -17157,7 +17173,7 @@
         <v>71</v>
       </c>
       <c r="B296" s="17" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -17169,7 +17185,7 @@
         <v>66</v>
       </c>
       <c r="B298" s="20" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -17209,7 +17225,7 @@
         <v>70</v>
       </c>
       <c r="B303" s="17" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -17217,7 +17233,7 @@
         <v>71</v>
       </c>
       <c r="B304" s="17" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -17225,7 +17241,7 @@
         <v>66</v>
       </c>
       <c r="B306" s="20" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -17265,7 +17281,7 @@
         <v>70</v>
       </c>
       <c r="B311" s="17" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="312" spans="1:2">
@@ -17273,7 +17289,7 @@
         <v>71</v>
       </c>
       <c r="B312" s="17" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -17281,7 +17297,7 @@
         <v>66</v>
       </c>
       <c r="B314" s="20" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -17321,7 +17337,7 @@
         <v>70</v>
       </c>
       <c r="B319" s="17" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -17329,7 +17345,7 @@
         <v>71</v>
       </c>
       <c r="B320" s="17" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -17973,7 +17989,7 @@
         <v>66</v>
       </c>
       <c r="B411" s="20" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
     </row>
     <row r="412" spans="1:2">
@@ -17989,7 +18005,7 @@
         <v>82</v>
       </c>
       <c r="B413" s="17" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="414" spans="1:2">
@@ -17997,7 +18013,7 @@
         <v>68</v>
       </c>
       <c r="B414" s="17" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="415" spans="1:2">
@@ -18013,7 +18029,7 @@
         <v>70</v>
       </c>
       <c r="B416" s="17" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="417" spans="1:2">
@@ -18021,7 +18037,7 @@
         <v>71</v>
       </c>
       <c r="B417" s="17" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="418" spans="1:2">
@@ -18033,7 +18049,7 @@
         <v>66</v>
       </c>
       <c r="B419" s="20" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
     <row r="420" spans="1:2">
@@ -18049,7 +18065,7 @@
         <v>82</v>
       </c>
       <c r="B421" s="17" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="422" spans="1:2">
@@ -18057,7 +18073,7 @@
         <v>68</v>
       </c>
       <c r="B422" s="17" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="423" spans="1:2">
@@ -18073,7 +18089,7 @@
         <v>70</v>
       </c>
       <c r="B424" s="17" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="425" spans="1:2">
@@ -18081,7 +18097,7 @@
         <v>71</v>
       </c>
       <c r="B425" s="17" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="427" spans="1:2">
@@ -18089,7 +18105,7 @@
         <v>66</v>
       </c>
       <c r="B427" s="20" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="428" spans="1:2">
@@ -18105,7 +18121,7 @@
         <v>82</v>
       </c>
       <c r="B429" s="17" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="430" spans="1:2">
@@ -18113,7 +18129,7 @@
         <v>68</v>
       </c>
       <c r="B430" s="17" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="431" spans="1:2">
@@ -18129,7 +18145,7 @@
         <v>70</v>
       </c>
       <c r="B432" s="17" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="433" spans="1:2">
@@ -18137,7 +18153,7 @@
         <v>71</v>
       </c>
       <c r="B433" s="17" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
     </row>
     <row r="435" spans="1:2">
@@ -18145,7 +18161,7 @@
         <v>66</v>
       </c>
       <c r="B435" s="20" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="436" spans="1:2">
@@ -18161,7 +18177,7 @@
         <v>82</v>
       </c>
       <c r="B437" s="17" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="438" spans="1:2">
@@ -18169,7 +18185,7 @@
         <v>68</v>
       </c>
       <c r="B438" s="17" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="439" spans="1:2">
@@ -18185,7 +18201,7 @@
         <v>70</v>
       </c>
       <c r="B440" s="17" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="441" spans="1:2">
@@ -18193,7 +18209,7 @@
         <v>71</v>
       </c>
       <c r="B441" s="17" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="443" spans="1:2">
@@ -18201,7 +18217,7 @@
         <v>66</v>
       </c>
       <c r="B443" s="20" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="444" spans="1:2">
@@ -18217,7 +18233,7 @@
         <v>82</v>
       </c>
       <c r="B445" s="17" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="446" spans="1:2">
@@ -18225,7 +18241,7 @@
         <v>68</v>
       </c>
       <c r="B446" s="17" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="447" spans="1:2">
@@ -18241,7 +18257,7 @@
         <v>70</v>
       </c>
       <c r="B448" s="17" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="449" spans="1:2">
@@ -18249,7 +18265,7 @@
         <v>71</v>
       </c>
       <c r="B449" s="17" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="450" spans="1:2">
@@ -18261,7 +18277,7 @@
         <v>66</v>
       </c>
       <c r="B451" s="20" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="452" spans="1:2">
@@ -18277,7 +18293,7 @@
         <v>82</v>
       </c>
       <c r="B453" s="17" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="454" spans="1:2">
@@ -18285,7 +18301,7 @@
         <v>68</v>
       </c>
       <c r="B454" s="17" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="455" spans="1:2">
@@ -18301,7 +18317,7 @@
         <v>70</v>
       </c>
       <c r="B456" s="17" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="457" spans="1:2">
@@ -18309,7 +18325,7 @@
         <v>71</v>
       </c>
       <c r="B457" s="17" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="459" spans="1:2">
@@ -18317,7 +18333,7 @@
         <v>66</v>
       </c>
       <c r="B459" s="20" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="460" spans="1:2">
@@ -18333,7 +18349,7 @@
         <v>82</v>
       </c>
       <c r="B461" s="17" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="462" spans="1:2">
@@ -18341,7 +18357,7 @@
         <v>68</v>
       </c>
       <c r="B462" s="17" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="463" spans="1:2">
@@ -18357,7 +18373,7 @@
         <v>70</v>
       </c>
       <c r="B464" s="17" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="465" spans="1:2">
@@ -18365,7 +18381,7 @@
         <v>71</v>
       </c>
       <c r="B465" s="17" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="467" spans="1:2">
@@ -18373,7 +18389,7 @@
         <v>66</v>
       </c>
       <c r="B467" s="20" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="468" spans="1:2">
@@ -18389,7 +18405,7 @@
         <v>82</v>
       </c>
       <c r="B469" s="17" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="470" spans="1:2">
@@ -18397,7 +18413,7 @@
         <v>68</v>
       </c>
       <c r="B470" s="17" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="471" spans="1:2">
@@ -18413,7 +18429,7 @@
         <v>70</v>
       </c>
       <c r="B472" s="17" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="473" spans="1:2">
@@ -18421,7 +18437,7 @@
         <v>71</v>
       </c>
       <c r="B473" s="17" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test cases and add logo to registration page
</commit_message>
<xml_diff>
--- a/test/client/e2e test cases.xlsx
+++ b/test/client/e2e test cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20300" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20300" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="未登录" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="设置" sheetId="9" r:id="rId7"/>
     <sheet name="面试" sheetId="10" r:id="rId8"/>
     <sheet name="pagination" sheetId="12" r:id="rId9"/>
+    <sheet name="面试设置" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3406" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="804">
   <si>
     <t>步骤</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3053,6 +3054,84 @@
   </si>
   <si>
     <t>该应聘者被放入人才库中，页面载入下一个简历，并回到页面顶部。导航栏中“通过”子菜单计数值减一。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting eventsetting 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/settings/eventsetting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击设置菜单，点击面试设置子菜单,在默认时长输入框中输入90。创建一个面试预约</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建面试预约对话框中，时长应默认为90</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮件被发送到应聘者邮箱。邮件模板中的姓名，应聘职位，开始时间和结束时间应被正确填写。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting eventsetting 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting eventsetting 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮件被发送到所有面试官邮箱。邮件模板中的姓名，应聘职位，开始时间和结束时间应被正确填写。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击设置菜单，点击面试设置子菜单,在创建面试邀请tab中勾选“当创建面试邀请时，自动发送邮件提醒给应聘者”。创建一个面试邀请，点击确定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击设置菜单，点击面试设置子菜单,在创建面试邀请tab中勾选“当创建面试邀请时，自动发送邮件提醒给面试官”。创建一个面试邀请，点击确定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting eventsetting 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting eventsetting 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮件模板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击设置菜单，点击面试设置子菜单,在修改面试邀请tab中勾选“当修改面试邀请时，自动发送邮件提醒给应聘者”。修改一个面试邀请，点击确定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting eventsetting 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting eventsetting 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在导航栏中点击设置菜单，点击面试设置子菜单,在取消面试邀请tab中勾选“当取消面试邀请时，自动发送邮件提醒给应聘者”。取消一个面试邀请，点击确定</t>
+  </si>
+  <si>
+    <t>在导航栏中点击设置菜单，点击面试设置子菜单,在创建面试邀请tab中勾选“当取消面试邀请时，自动发送邮件提醒给面试官”。取消一个面试邀请，点击确定</t>
+  </si>
+  <si>
+    <t>在导航栏中点击设置菜单，点击面试设置子菜单,在修改面试邀请tab中勾选“当修改面试邀请时，自动发送邮件提醒给面试官”。修改一个面试邀请，点击确定</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3195,8 +3274,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="703">
+  <cellStyleXfs count="733">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3966,7 +4075,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="703">
+  <cellStyles count="733">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -4318,6 +4427,21 @@
     <cellStyle name="超链接" xfId="697" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="699" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="731" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -4669,6 +4793,21 @@
     <cellStyle name="访问过的超链接" xfId="698" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="700" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="732" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5706,6 +5845,424 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30">
+      <c r="A6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="45">
+      <c r="A14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30">
+      <c r="A15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="45">
+      <c r="A22" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30">
+      <c r="A23" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="45">
+      <c r="A30" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="30">
+      <c r="A31" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="45">
+      <c r="A38" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="30">
+      <c r="A39" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="45">
+      <c r="A46" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30">
+      <c r="A47" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="45">
+      <c r="A54" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="30">
+      <c r="A55" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B84"/>
@@ -6360,7 +6917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A362" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="A362" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="F376" sqref="F376"/>
     </sheetView>
   </sheetViews>
@@ -9155,7 +9712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B336"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
       <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
@@ -15066,7 +15623,7 @@
   <dimension ref="A1:B473"/>
   <sheetViews>
     <sheetView topLeftCell="A444" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="C453" sqref="C453"/>
+      <selection activeCell="A467" sqref="A467:B472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18457,7 +19014,7 @@
   <dimension ref="A1:B87"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A15" sqref="A15:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>